<commit_message>
retrained of some 5verbs experiments
</commit_message>
<xml_diff>
--- a/ExperimentosJoe.xlsx
+++ b/ExperimentosJoe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Projects\PeruvianSignLanguage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8336EDC9-5E88-486B-B870-B39795512395}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{766558E6-09D7-4D3C-8734-769220033461}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{B664CC47-0CDC-4C29-8327-B2D4CD6615DF}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="26">
   <si>
     <t>10nouns</t>
   </si>
@@ -108,12 +108,15 @@
   <si>
     <t>5verbs</t>
   </si>
+  <si>
+    <t>5verbs - retrained</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,8 +130,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -138,6 +149,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -154,10 +171,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,17 +491,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98E7DA79-1D56-4C42-82B7-A2573CE01401}">
-  <dimension ref="A1:P38"/>
+  <dimension ref="A1:P46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P33" sqref="P33"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="3" width="11" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
     <col min="4" max="4" width="14.140625" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" customWidth="1"/>
     <col min="11" max="11" width="13" bestFit="1" customWidth="1"/>
@@ -2074,7 +2094,7 @@
         <v>0.48507462686567099</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -2120,8 +2140,9 @@
       <c r="O33">
         <v>0.29850746268656703</v>
       </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P33" s="3"/>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>19</v>
       </c>
@@ -2168,7 +2189,7 @@
         <v>0.51492537313432796</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>19</v>
       </c>
@@ -2215,7 +2236,7 @@
         <v>0.201492537313432</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>19</v>
       </c>
@@ -2262,7 +2283,7 @@
         <v>0.63432835820895495</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>19</v>
       </c>
@@ -2309,7 +2330,7 @@
         <v>9.7014925373134303E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>19</v>
       </c>
@@ -2355,6 +2376,201 @@
       <c r="O38">
         <v>0.64179104477611904</v>
       </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B40" t="s">
+        <v>25</v>
+      </c>
+      <c r="C40">
+        <v>54</v>
+      </c>
+      <c r="D40">
+        <v>10</v>
+      </c>
+      <c r="E40" t="s">
+        <v>14</v>
+      </c>
+      <c r="F40">
+        <v>100</v>
+      </c>
+      <c r="G40">
+        <v>1</v>
+      </c>
+      <c r="H40">
+        <v>8</v>
+      </c>
+      <c r="I40">
+        <v>8</v>
+      </c>
+      <c r="J40">
+        <v>0</v>
+      </c>
+      <c r="K40">
+        <v>0.1188</v>
+      </c>
+      <c r="L40">
+        <v>1</v>
+      </c>
+      <c r="M40">
+        <v>0.41389999999999999</v>
+      </c>
+      <c r="N40">
+        <v>0.86960000000000004</v>
+      </c>
+      <c r="O40">
+        <v>0.21641791044776101</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B41" t="s">
+        <v>25</v>
+      </c>
+      <c r="C41">
+        <v>55</v>
+      </c>
+      <c r="D41">
+        <v>10</v>
+      </c>
+      <c r="E41" t="s">
+        <v>7</v>
+      </c>
+      <c r="F41">
+        <v>100</v>
+      </c>
+      <c r="G41">
+        <v>1</v>
+      </c>
+      <c r="H41">
+        <v>8</v>
+      </c>
+      <c r="I41">
+        <v>8</v>
+      </c>
+      <c r="J41">
+        <v>0</v>
+      </c>
+      <c r="K41">
+        <v>1.1040000000000001</v>
+      </c>
+      <c r="L41">
+        <v>0.72629999999999995</v>
+      </c>
+      <c r="M41">
+        <v>1.2490000000000001</v>
+      </c>
+      <c r="N41">
+        <v>0.52170000000000005</v>
+      </c>
+      <c r="O41">
+        <v>0.57462686567164101</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B42" t="s">
+        <v>25</v>
+      </c>
+      <c r="C42">
+        <v>56</v>
+      </c>
+      <c r="D42" s="3">
+        <v>10</v>
+      </c>
+      <c r="E42" t="s">
+        <v>14</v>
+      </c>
+      <c r="F42">
+        <v>100</v>
+      </c>
+      <c r="G42">
+        <v>2</v>
+      </c>
+      <c r="H42">
+        <v>8</v>
+      </c>
+      <c r="I42">
+        <v>8</v>
+      </c>
+      <c r="J42">
+        <v>0</v>
+      </c>
+      <c r="K42">
+        <v>0.22869999999999999</v>
+      </c>
+      <c r="L42">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="M42">
+        <v>0.48249999999999998</v>
+      </c>
+      <c r="N42">
+        <v>0.86960000000000004</v>
+      </c>
+      <c r="O42">
+        <v>0.29104477611940299</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B43" t="s">
+        <v>25</v>
+      </c>
+      <c r="C43">
+        <v>57</v>
+      </c>
+      <c r="D43">
+        <v>10</v>
+      </c>
+      <c r="E43" t="s">
+        <v>7</v>
+      </c>
+      <c r="F43">
+        <v>100</v>
+      </c>
+      <c r="G43">
+        <v>2</v>
+      </c>
+      <c r="H43">
+        <v>8</v>
+      </c>
+      <c r="I43">
+        <v>8</v>
+      </c>
+      <c r="J43">
+        <v>0</v>
+      </c>
+      <c r="K43">
+        <v>1.1679999999999999</v>
+      </c>
+      <c r="L43">
+        <v>0.70330000000000004</v>
+      </c>
+      <c r="M43">
+        <v>1.302</v>
+      </c>
+      <c r="N43">
+        <v>0.4783</v>
+      </c>
+      <c r="O43">
+        <v>0.56716417910447703</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E45" s="2"/>
+      <c r="N45" s="3"/>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D46" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
e-6 in experiments Joe
</commit_message>
<xml_diff>
--- a/ExperimentosJoe.xlsx
+++ b/ExperimentosJoe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Projects\PeruvianSignLanguage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{766558E6-09D7-4D3C-8734-769220033461}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FAA7F85-644A-4256-9812-1D3D424AA018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{B664CC47-0CDC-4C29-8327-B2D4CD6615DF}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="26">
   <si>
     <t>10nouns</t>
   </si>
@@ -493,9 +493,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98E7DA79-1D56-4C42-82B7-A2573CE01401}">
   <dimension ref="A1:P46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E45" sqref="E45"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K49" sqref="K49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2565,9 +2565,99 @@
         <v>0.56716417910447703</v>
       </c>
     </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B44" t="s">
+        <v>25</v>
+      </c>
+      <c r="C44">
+        <v>58</v>
+      </c>
+      <c r="D44">
+        <v>10</v>
+      </c>
+      <c r="E44" t="s">
+        <v>8</v>
+      </c>
+      <c r="F44">
+        <v>100</v>
+      </c>
+      <c r="G44">
+        <v>2</v>
+      </c>
+      <c r="H44">
+        <v>8</v>
+      </c>
+      <c r="I44">
+        <v>8</v>
+      </c>
+      <c r="J44">
+        <v>0</v>
+      </c>
+      <c r="K44">
+        <v>1.518</v>
+      </c>
+      <c r="L44">
+        <v>0.3846</v>
+      </c>
+      <c r="M44">
+        <v>1.573</v>
+      </c>
+      <c r="N44">
+        <v>0.26090000000000002</v>
+      </c>
+      <c r="O44">
+        <v>0.62686567164179097</v>
+      </c>
+    </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="E45" s="2"/>
-      <c r="N45" s="3"/>
+      <c r="A45" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B45" t="s">
+        <v>25</v>
+      </c>
+      <c r="C45">
+        <v>59</v>
+      </c>
+      <c r="D45">
+        <v>10</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F45">
+        <v>100</v>
+      </c>
+      <c r="G45">
+        <v>1</v>
+      </c>
+      <c r="H45">
+        <v>8</v>
+      </c>
+      <c r="I45">
+        <v>8</v>
+      </c>
+      <c r="J45">
+        <v>0</v>
+      </c>
+      <c r="K45">
+        <v>1.5109999999999999</v>
+      </c>
+      <c r="L45">
+        <v>0.3846</v>
+      </c>
+      <c r="M45">
+        <v>1.302</v>
+      </c>
+      <c r="N45" s="2">
+        <v>0.4783</v>
+      </c>
+      <c r="O45">
+        <v>0.63432835820895495</v>
+      </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D46" s="3"/>

</xml_diff>

<commit_message>
experiments with 15 words - joe
</commit_message>
<xml_diff>
--- a/ExperimentosJoe.xlsx
+++ b/ExperimentosJoe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Projects\PeruvianSignLanguage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FAA7F85-644A-4256-9812-1D3D424AA018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2C4781E-44B4-45B2-ADE1-857F75DC28BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{B664CC47-0CDC-4C29-8327-B2D4CD6615DF}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="27">
   <si>
     <t>10nouns</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>5verbs - retrained</t>
+  </si>
+  <si>
+    <t>15words</t>
   </si>
 </sst>
 </file>
@@ -491,11 +494,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98E7DA79-1D56-4C42-82B7-A2573CE01401}">
-  <dimension ref="A1:P46"/>
+  <dimension ref="A1:P62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K49" sqref="K49"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K65" sqref="K65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2377,6 +2380,50 @@
         <v>0.64179104477611904</v>
       </c>
     </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>25</v>
+      </c>
+      <c r="C39">
+        <v>54</v>
+      </c>
+      <c r="D39">
+        <v>10</v>
+      </c>
+      <c r="E39" t="s">
+        <v>14</v>
+      </c>
+      <c r="F39">
+        <v>100</v>
+      </c>
+      <c r="G39">
+        <v>1</v>
+      </c>
+      <c r="H39">
+        <v>8</v>
+      </c>
+      <c r="I39">
+        <v>8</v>
+      </c>
+      <c r="J39">
+        <v>0</v>
+      </c>
+      <c r="K39">
+        <v>0.1188</v>
+      </c>
+      <c r="L39">
+        <v>1</v>
+      </c>
+      <c r="M39">
+        <v>0.41389999999999999</v>
+      </c>
+      <c r="N39">
+        <v>0.86960000000000004</v>
+      </c>
+      <c r="O39">
+        <v>0.21641791044776101</v>
+      </c>
+    </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>19</v>
@@ -2385,13 +2432,13 @@
         <v>25</v>
       </c>
       <c r="C40">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D40">
         <v>10</v>
       </c>
       <c r="E40" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F40">
         <v>100</v>
@@ -2409,19 +2456,19 @@
         <v>0</v>
       </c>
       <c r="K40">
-        <v>0.1188</v>
+        <v>1.1040000000000001</v>
       </c>
       <c r="L40">
-        <v>1</v>
+        <v>0.72629999999999995</v>
       </c>
       <c r="M40">
-        <v>0.41389999999999999</v>
+        <v>1.2490000000000001</v>
       </c>
       <c r="N40">
-        <v>0.86960000000000004</v>
+        <v>0.52170000000000005</v>
       </c>
       <c r="O40">
-        <v>0.21641791044776101</v>
+        <v>0.57462686567164101</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
@@ -2432,19 +2479,19 @@
         <v>25</v>
       </c>
       <c r="C41">
-        <v>55</v>
-      </c>
-      <c r="D41">
+        <v>56</v>
+      </c>
+      <c r="D41" s="3">
         <v>10</v>
       </c>
       <c r="E41" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F41">
         <v>100</v>
       </c>
       <c r="G41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H41">
         <v>8</v>
@@ -2456,19 +2503,19 @@
         <v>0</v>
       </c>
       <c r="K41">
-        <v>1.1040000000000001</v>
+        <v>0.22869999999999999</v>
       </c>
       <c r="L41">
-        <v>0.72629999999999995</v>
+        <v>0.98899999999999999</v>
       </c>
       <c r="M41">
-        <v>1.2490000000000001</v>
+        <v>0.48249999999999998</v>
       </c>
       <c r="N41">
-        <v>0.52170000000000005</v>
+        <v>0.86960000000000004</v>
       </c>
       <c r="O41">
-        <v>0.57462686567164101</v>
+        <v>0.29104477611940299</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
@@ -2479,13 +2526,13 @@
         <v>25</v>
       </c>
       <c r="C42">
-        <v>56</v>
-      </c>
-      <c r="D42" s="3">
+        <v>57</v>
+      </c>
+      <c r="D42">
         <v>10</v>
       </c>
       <c r="E42" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F42">
         <v>100</v>
@@ -2503,19 +2550,19 @@
         <v>0</v>
       </c>
       <c r="K42">
-        <v>0.22869999999999999</v>
+        <v>1.1679999999999999</v>
       </c>
       <c r="L42">
-        <v>0.98899999999999999</v>
+        <v>0.70330000000000004</v>
       </c>
       <c r="M42">
-        <v>0.48249999999999998</v>
+        <v>1.302</v>
       </c>
       <c r="N42">
-        <v>0.86960000000000004</v>
+        <v>0.4783</v>
       </c>
       <c r="O42">
-        <v>0.29104477611940299</v>
+        <v>0.56716417910447703</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
@@ -2526,13 +2573,13 @@
         <v>25</v>
       </c>
       <c r="C43">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D43">
         <v>10</v>
       </c>
       <c r="E43" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F43">
         <v>100</v>
@@ -2550,19 +2597,19 @@
         <v>0</v>
       </c>
       <c r="K43">
-        <v>1.1679999999999999</v>
+        <v>1.518</v>
       </c>
       <c r="L43">
-        <v>0.70330000000000004</v>
+        <v>0.3846</v>
       </c>
       <c r="M43">
-        <v>1.302</v>
+        <v>1.573</v>
       </c>
       <c r="N43">
-        <v>0.4783</v>
+        <v>0.26090000000000002</v>
       </c>
       <c r="O43">
-        <v>0.56716417910447703</v>
+        <v>0.62686567164179097</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
@@ -2573,19 +2620,19 @@
         <v>25</v>
       </c>
       <c r="C44">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D44">
         <v>10</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E44" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F44">
         <v>100</v>
       </c>
       <c r="G44">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H44">
         <v>8</v>
@@ -2597,19 +2644,19 @@
         <v>0</v>
       </c>
       <c r="K44">
-        <v>1.518</v>
+        <v>1.5109999999999999</v>
       </c>
       <c r="L44">
         <v>0.3846</v>
       </c>
       <c r="M44">
-        <v>1.573</v>
-      </c>
-      <c r="N44">
-        <v>0.26090000000000002</v>
+        <v>1.302</v>
+      </c>
+      <c r="N44" s="2">
+        <v>0.4783</v>
       </c>
       <c r="O44">
-        <v>0.62686567164179097</v>
+        <v>0.63432835820895495</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
@@ -2617,10 +2664,10 @@
         <v>19</v>
       </c>
       <c r="B45" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C45">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D45">
         <v>10</v>
@@ -2632,35 +2679,780 @@
         <v>100</v>
       </c>
       <c r="G45">
+        <v>2</v>
+      </c>
+      <c r="H45">
+        <v>8</v>
+      </c>
+      <c r="I45">
+        <v>8</v>
+      </c>
+      <c r="J45">
+        <v>0</v>
+      </c>
+      <c r="K45">
+        <v>0.25619999999999998</v>
+      </c>
+      <c r="L45">
+        <v>0.1905</v>
+      </c>
+      <c r="M45">
+        <v>2.617</v>
+      </c>
+      <c r="N45" s="2">
+        <v>0.1905</v>
+      </c>
+      <c r="O45">
+        <v>0.15730337078651599</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>26</v>
+      </c>
+      <c r="C46">
+        <v>64</v>
+      </c>
+      <c r="D46">
+        <v>10</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F46">
+        <v>100</v>
+      </c>
+      <c r="G46">
         <v>1</v>
       </c>
-      <c r="H45">
-        <v>8</v>
-      </c>
-      <c r="I45">
-        <v>8</v>
-      </c>
-      <c r="J45">
-        <v>0</v>
-      </c>
-      <c r="K45">
-        <v>1.5109999999999999</v>
-      </c>
-      <c r="L45">
-        <v>0.3846</v>
-      </c>
-      <c r="M45">
-        <v>1.302</v>
-      </c>
-      <c r="N45" s="2">
-        <v>0.4783</v>
-      </c>
-      <c r="O45">
-        <v>0.63432835820895495</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D46" s="3"/>
+      <c r="H46">
+        <v>8</v>
+      </c>
+      <c r="I46">
+        <v>8</v>
+      </c>
+      <c r="J46">
+        <v>0</v>
+      </c>
+      <c r="K46">
+        <v>2.5430000000000001</v>
+      </c>
+      <c r="L46">
+        <v>0.1905</v>
+      </c>
+      <c r="M46">
+        <v>2.6150000000000002</v>
+      </c>
+      <c r="N46" s="2">
+        <v>0.17460000000000001</v>
+      </c>
+      <c r="O46">
+        <v>0.14606741573033699</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>26</v>
+      </c>
+      <c r="C47">
+        <v>65</v>
+      </c>
+      <c r="D47">
+        <v>10</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F47">
+        <v>100</v>
+      </c>
+      <c r="G47">
+        <v>2</v>
+      </c>
+      <c r="H47">
+        <v>8</v>
+      </c>
+      <c r="I47">
+        <v>8</v>
+      </c>
+      <c r="J47">
+        <v>0</v>
+      </c>
+      <c r="K47">
+        <v>2.15</v>
+      </c>
+      <c r="L47">
+        <v>0.38100000000000001</v>
+      </c>
+      <c r="M47">
+        <v>2.3210000000000002</v>
+      </c>
+      <c r="N47" s="2">
+        <v>0.28570000000000001</v>
+      </c>
+      <c r="O47">
+        <v>0.188202247191011</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>26</v>
+      </c>
+      <c r="C48">
+        <v>66</v>
+      </c>
+      <c r="D48">
+        <v>10</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F48">
+        <v>100</v>
+      </c>
+      <c r="G48">
+        <v>1</v>
+      </c>
+      <c r="H48">
+        <v>8</v>
+      </c>
+      <c r="I48">
+        <v>8</v>
+      </c>
+      <c r="J48">
+        <v>0</v>
+      </c>
+      <c r="K48">
+        <v>2.1320000000000001</v>
+      </c>
+      <c r="L48">
+        <v>0.39290000000000003</v>
+      </c>
+      <c r="M48">
+        <v>2.274</v>
+      </c>
+      <c r="N48" s="2">
+        <v>0.3175</v>
+      </c>
+      <c r="O48">
+        <v>0.199438202247191</v>
+      </c>
+    </row>
+    <row r="49" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>26</v>
+      </c>
+      <c r="C49">
+        <v>67</v>
+      </c>
+      <c r="D49">
+        <v>10</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F49">
+        <v>100</v>
+      </c>
+      <c r="G49">
+        <v>2</v>
+      </c>
+      <c r="H49">
+        <v>8</v>
+      </c>
+      <c r="I49">
+        <v>8</v>
+      </c>
+      <c r="J49">
+        <v>0</v>
+      </c>
+      <c r="K49">
+        <v>0.3044</v>
+      </c>
+      <c r="L49">
+        <v>0.94440000000000002</v>
+      </c>
+      <c r="M49">
+        <v>0.87119999999999997</v>
+      </c>
+      <c r="N49" s="2">
+        <v>0.76190000000000002</v>
+      </c>
+      <c r="O49">
+        <v>0.13483146067415699</v>
+      </c>
+    </row>
+    <row r="50" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>26</v>
+      </c>
+      <c r="C50">
+        <v>68</v>
+      </c>
+      <c r="D50">
+        <v>10</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F50">
+        <v>100</v>
+      </c>
+      <c r="G50">
+        <v>1</v>
+      </c>
+      <c r="H50">
+        <v>8</v>
+      </c>
+      <c r="I50">
+        <v>8</v>
+      </c>
+      <c r="J50">
+        <v>0</v>
+      </c>
+      <c r="K50">
+        <v>0.2243</v>
+      </c>
+      <c r="L50">
+        <v>0.96430000000000005</v>
+      </c>
+      <c r="M50">
+        <v>0.875</v>
+      </c>
+      <c r="N50" s="2">
+        <v>0.77780000000000005</v>
+      </c>
+      <c r="O50">
+        <v>0.117977528089887</v>
+      </c>
+    </row>
+    <row r="51" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>26</v>
+      </c>
+      <c r="C51">
+        <v>69</v>
+      </c>
+      <c r="D51">
+        <v>15</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F51">
+        <v>100</v>
+      </c>
+      <c r="G51">
+        <v>2</v>
+      </c>
+      <c r="H51">
+        <v>8</v>
+      </c>
+      <c r="I51">
+        <v>8</v>
+      </c>
+      <c r="J51">
+        <v>0</v>
+      </c>
+      <c r="K51">
+        <v>2.5590000000000002</v>
+      </c>
+      <c r="L51">
+        <v>0.1825</v>
+      </c>
+      <c r="M51">
+        <v>2.5409999999999999</v>
+      </c>
+      <c r="N51" s="2">
+        <v>0.1905</v>
+      </c>
+      <c r="O51">
+        <v>0.101123595505617</v>
+      </c>
+    </row>
+    <row r="52" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>26</v>
+      </c>
+      <c r="C52">
+        <v>70</v>
+      </c>
+      <c r="D52">
+        <v>15</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F52">
+        <v>100</v>
+      </c>
+      <c r="G52">
+        <v>1</v>
+      </c>
+      <c r="H52">
+        <v>8</v>
+      </c>
+      <c r="I52">
+        <v>8</v>
+      </c>
+      <c r="J52">
+        <v>0</v>
+      </c>
+      <c r="K52">
+        <v>2.54</v>
+      </c>
+      <c r="L52">
+        <v>0.1905</v>
+      </c>
+      <c r="M52">
+        <v>2.5379999999999998</v>
+      </c>
+      <c r="N52" s="2">
+        <v>0.1905</v>
+      </c>
+      <c r="O52">
+        <v>0.101123595505617</v>
+      </c>
+    </row>
+    <row r="53" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>26</v>
+      </c>
+      <c r="C53">
+        <v>71</v>
+      </c>
+      <c r="D53">
+        <v>15</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F53">
+        <v>100</v>
+      </c>
+      <c r="G53">
+        <v>2</v>
+      </c>
+      <c r="H53">
+        <v>8</v>
+      </c>
+      <c r="I53">
+        <v>8</v>
+      </c>
+      <c r="J53">
+        <v>0</v>
+      </c>
+      <c r="K53">
+        <v>2.1880000000000002</v>
+      </c>
+      <c r="L53">
+        <v>0.38100000000000001</v>
+      </c>
+      <c r="M53">
+        <v>2.2789999999999999</v>
+      </c>
+      <c r="N53" s="2">
+        <v>0.3175</v>
+      </c>
+      <c r="O53">
+        <v>0.123595505617977</v>
+      </c>
+    </row>
+    <row r="54" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>26</v>
+      </c>
+      <c r="C54">
+        <v>72</v>
+      </c>
+      <c r="D54">
+        <v>15</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F54">
+        <v>100</v>
+      </c>
+      <c r="G54">
+        <v>1</v>
+      </c>
+      <c r="H54">
+        <v>8</v>
+      </c>
+      <c r="I54">
+        <v>8</v>
+      </c>
+      <c r="J54">
+        <v>0</v>
+      </c>
+      <c r="K54">
+        <v>2.137</v>
+      </c>
+      <c r="L54">
+        <v>0.40079999999999999</v>
+      </c>
+      <c r="M54">
+        <v>2.2349999999999999</v>
+      </c>
+      <c r="N54" s="2">
+        <v>0.38100000000000001</v>
+      </c>
+      <c r="O54">
+        <v>0.148876404494382</v>
+      </c>
+    </row>
+    <row r="55" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>26</v>
+      </c>
+      <c r="C55">
+        <v>73</v>
+      </c>
+      <c r="D55">
+        <v>15</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F55">
+        <v>100</v>
+      </c>
+      <c r="G55">
+        <v>2</v>
+      </c>
+      <c r="H55">
+        <v>8</v>
+      </c>
+      <c r="I55">
+        <v>8</v>
+      </c>
+      <c r="J55">
+        <v>0</v>
+      </c>
+      <c r="K55">
+        <v>0.36270000000000002</v>
+      </c>
+      <c r="L55">
+        <v>0.92459999999999998</v>
+      </c>
+      <c r="M55">
+        <v>0.99209999999999998</v>
+      </c>
+      <c r="N55" s="2">
+        <v>0.6825</v>
+      </c>
+      <c r="O55">
+        <v>0.12921348314606701</v>
+      </c>
+    </row>
+    <row r="56" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>26</v>
+      </c>
+      <c r="C56">
+        <v>74</v>
+      </c>
+      <c r="D56">
+        <v>15</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F56">
+        <v>100</v>
+      </c>
+      <c r="G56">
+        <v>1</v>
+      </c>
+      <c r="H56">
+        <v>8</v>
+      </c>
+      <c r="I56">
+        <v>8</v>
+      </c>
+      <c r="J56">
+        <v>0</v>
+      </c>
+      <c r="K56">
+        <v>0.2792</v>
+      </c>
+      <c r="L56">
+        <v>0.96030000000000004</v>
+      </c>
+      <c r="M56">
+        <v>0.747</v>
+      </c>
+      <c r="N56">
+        <v>0.73019999999999996</v>
+      </c>
+      <c r="O56">
+        <v>0.106741573033707</v>
+      </c>
+    </row>
+    <row r="57" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>26</v>
+      </c>
+      <c r="C57">
+        <v>75</v>
+      </c>
+      <c r="D57">
+        <v>20</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F57">
+        <v>100</v>
+      </c>
+      <c r="G57">
+        <v>2</v>
+      </c>
+      <c r="H57">
+        <v>8</v>
+      </c>
+      <c r="I57">
+        <v>8</v>
+      </c>
+      <c r="J57">
+        <v>0</v>
+      </c>
+      <c r="K57">
+        <v>2.5390000000000001</v>
+      </c>
+      <c r="L57">
+        <v>0.1905</v>
+      </c>
+      <c r="M57">
+        <v>2.5830000000000002</v>
+      </c>
+      <c r="N57">
+        <v>0.17460000000000001</v>
+      </c>
+      <c r="O57">
+        <v>0.19382022471910099</v>
+      </c>
+    </row>
+    <row r="58" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>26</v>
+      </c>
+      <c r="C58">
+        <v>76</v>
+      </c>
+      <c r="D58">
+        <v>20</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F58">
+        <v>100</v>
+      </c>
+      <c r="G58">
+        <v>1</v>
+      </c>
+      <c r="H58">
+        <v>8</v>
+      </c>
+      <c r="I58">
+        <v>8</v>
+      </c>
+      <c r="J58">
+        <v>0</v>
+      </c>
+      <c r="K58">
+        <v>2.5409999999999999</v>
+      </c>
+      <c r="L58">
+        <v>0.1905</v>
+      </c>
+      <c r="M58">
+        <v>2.5710000000000002</v>
+      </c>
+      <c r="N58">
+        <v>0.1905</v>
+      </c>
+      <c r="O58">
+        <v>0.174157303370786</v>
+      </c>
+    </row>
+    <row r="59" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>26</v>
+      </c>
+      <c r="C59">
+        <v>77</v>
+      </c>
+      <c r="D59">
+        <v>20</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F59">
+        <v>100</v>
+      </c>
+      <c r="G59">
+        <v>2</v>
+      </c>
+      <c r="H59">
+        <v>8</v>
+      </c>
+      <c r="I59">
+        <v>8</v>
+      </c>
+      <c r="J59">
+        <v>0</v>
+      </c>
+      <c r="K59">
+        <v>2.1909999999999998</v>
+      </c>
+      <c r="L59">
+        <v>0.377</v>
+      </c>
+      <c r="M59">
+        <v>2.3220000000000001</v>
+      </c>
+      <c r="N59">
+        <v>0.26979999999999998</v>
+      </c>
+      <c r="O59">
+        <v>0.21067415730337</v>
+      </c>
+    </row>
+    <row r="60" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>26</v>
+      </c>
+      <c r="C60">
+        <v>78</v>
+      </c>
+      <c r="D60">
+        <v>20</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F60">
+        <v>100</v>
+      </c>
+      <c r="G60">
+        <v>1</v>
+      </c>
+      <c r="H60">
+        <v>8</v>
+      </c>
+      <c r="I60">
+        <v>8</v>
+      </c>
+      <c r="J60">
+        <v>0</v>
+      </c>
+      <c r="K60">
+        <v>2.1619999999999999</v>
+      </c>
+      <c r="L60">
+        <v>0.39679999999999999</v>
+      </c>
+      <c r="M60">
+        <v>2.2709999999999999</v>
+      </c>
+      <c r="N60">
+        <v>0.28570000000000001</v>
+      </c>
+      <c r="O60">
+        <v>0.21629213483146001</v>
+      </c>
+    </row>
+    <row r="61" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>26</v>
+      </c>
+      <c r="C61">
+        <v>79</v>
+      </c>
+      <c r="D61">
+        <v>20</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F61">
+        <v>100</v>
+      </c>
+      <c r="G61">
+        <v>2</v>
+      </c>
+      <c r="H61">
+        <v>8</v>
+      </c>
+      <c r="I61">
+        <v>8</v>
+      </c>
+      <c r="J61">
+        <v>0</v>
+      </c>
+      <c r="K61">
+        <v>0.38519999999999999</v>
+      </c>
+      <c r="L61">
+        <v>0.92859999999999998</v>
+      </c>
+      <c r="M61">
+        <v>1.1539999999999999</v>
+      </c>
+      <c r="N61">
+        <v>0.66669999999999996</v>
+      </c>
+      <c r="O61">
+        <v>0.13202247191011199</v>
+      </c>
+    </row>
+    <row r="62" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>26</v>
+      </c>
+      <c r="C62">
+        <v>80</v>
+      </c>
+      <c r="D62">
+        <v>20</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F62">
+        <v>100</v>
+      </c>
+      <c r="G62">
+        <v>1</v>
+      </c>
+      <c r="H62">
+        <v>8</v>
+      </c>
+      <c r="I62">
+        <v>8</v>
+      </c>
+      <c r="J62">
+        <v>0</v>
+      </c>
+      <c r="K62">
+        <v>0.30220000000000002</v>
+      </c>
+      <c r="L62">
+        <v>0.95030000000000003</v>
+      </c>
+      <c r="M62">
+        <v>0.85870000000000002</v>
+      </c>
+      <c r="N62" s="2">
+        <v>0.746</v>
+      </c>
+      <c r="O62">
+        <v>0.13483146067415699</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>